<commit_message>
Add new sheets with the inAppDeliveryCode
</commit_message>
<xml_diff>
--- a/template_recovery.xlsx
+++ b/template_recovery.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\REFERENCE_FILES_CSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cedricmoullet/sandbox/CovidCertificate-UIdoc/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4822DC8-E1B2-2E4B-B067-F4FC78114353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12465"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="recovery" sheetId="2" r:id="rId1"/>
     <sheet name="recovery_print" sheetId="1" r:id="rId2"/>
+    <sheet name="recovery_transfer" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>givenName</t>
   </si>
@@ -71,12 +73,18 @@
   </si>
   <si>
     <t>MüsterStrasse 1</t>
+  </si>
+  <si>
+    <t>inAppDeliveryCode</t>
+  </si>
+  <si>
+    <t>Y8P8ECFN8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -914,24 +922,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="1"/>
-    <col min="4" max="4" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -951,7 +959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -980,28 +988,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="1"/>
-    <col min="4" max="4" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1033,7 +1041,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1071,4 +1079,74 @@
     <customPr name="EpmWorksheetKeyString_GUID" r:id="rId1"/>
   </customProperties>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25571305-6024-C14D-8BE7-C7926CA8F413}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1">
+        <v>31310</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44344</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
+</worksheet>
 </file>
</xml_diff>